<commit_message>
Java Basics - completed
</commit_message>
<xml_diff>
--- a/glossary.xlsx
+++ b/glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6fc519bcb61589f5/Coding/JAVA/java-foundations-exam-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{CF536931-B1DA-8B48-9E91-234EB7219217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A10290D-3640-3946-BD1D-6D38CB1C7FB1}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{CF536931-B1DA-8B48-9E91-234EB7219217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7EEBAEF-C2B6-3347-AA08-B200B9D05678}"/>
   <bookViews>
     <workbookView xWindow="19940" yWindow="500" windowWidth="31260" windowHeight="28300" xr2:uid="{861D1597-45A4-5C48-8EB6-87737743CF3E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>Term</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>final</t>
   </si>
 </sst>
 </file>
@@ -1011,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BBFA876-2097-CB4B-91A6-045FF54B33B0}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1312,6 +1315,11 @@
         <v>74</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>